<commit_message>
Added files for integration tests
</commit_message>
<xml_diff>
--- a/src/test/resources/IntegrationTest.xlsx
+++ b/src/test/resources/IntegrationTest.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DEVIAPHAN\IdeaProjects\University\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA39A2DA-8CE2-47A3-8360-1CEF47149FF8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97EA7E42-4797-4A43-BBDD-6AF36C00A3B6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="9000" windowWidth="19200" windowHeight="6330" tabRatio="882" activeTab="2" xr2:uid="{6C53CB67-0793-4BD9-89E2-7181CFEEFA82}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="19440" windowHeight="15150" tabRatio="882" activeTab="2" xr2:uid="{6C53CB67-0793-4BD9-89E2-7181CFEEFA82}"/>
   </bookViews>
   <sheets>
     <sheet name="Зачисление в группу студента" sheetId="2" r:id="rId1"/>
-    <sheet name="Зачисление в группу студент (Р)" sheetId="9" r:id="rId2"/>
-    <sheet name="Группы у преподавателя" sheetId="7" r:id="rId3"/>
-    <sheet name="Группы у преподавателя (Р)" sheetId="10" r:id="rId4"/>
+    <sheet name="Группы у преподавателя" sheetId="7" r:id="rId2"/>
+    <sheet name="Группы у преподавателя (Р)" sheetId="10" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <t>ПОИТ-162</t>
   </si>
@@ -90,31 +89,13 @@
     <t>Группа №4</t>
   </si>
   <si>
-    <t>Lee</t>
-  </si>
-  <si>
-    <t>Walker</t>
-  </si>
-  <si>
     <t>POIT-161</t>
   </si>
   <si>
-    <t>Moore</t>
-  </si>
-  <si>
     <t>POIT-162</t>
   </si>
   <si>
-    <t>Lopez</t>
-  </si>
-  <si>
     <t>POIT-21</t>
-  </si>
-  <si>
-    <t>Levis</t>
-  </si>
-  <si>
-    <t>Bob</t>
   </si>
   <si>
     <t>Jackie</t>
@@ -572,76 +553,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44C36F4F-28C5-4E1B-922A-614AB5A42968}">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="31" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9014C1E-2E79-4753-A18F-EDF8D3733FDA}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,11 +631,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F9481D7-AE98-4EDC-8B45-51578EF0C851}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -755,41 +671,41 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>